<commit_message>
upd: refactoring and add some docstrings
</commit_message>
<xml_diff>
--- a/ITsleng_project/AppMetric - Events Map.xlsx
+++ b/ITsleng_project/AppMetric - Events Map.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TSuvorov_learing\AliceProjects\ITsleng_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TSuvorov_Projects\AliceProjects\ITsleng_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE44BD6E-447E-45DF-BDDC-35C12F8CD05D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1740111E-888B-4E60-B806-F404CDC3AE53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
   <si>
     <t>Триггер</t>
   </si>
@@ -173,6 +173,18 @@
   </si>
   <si>
     <t>Вне сценария c вопросом</t>
+  </si>
+  <si>
+    <t>Возникновение исключения</t>
+  </si>
+  <si>
+    <t>Ошибка в системе</t>
+  </si>
+  <si>
+    <t>текст ошибки</t>
+  </si>
+  <si>
+    <t>Возникла непредвиденная ошибка в одной из функций</t>
   </si>
 </sst>
 </file>
@@ -235,7 +247,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -485,11 +497,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -538,6 +589,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -756,10 +822,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E1001"/>
+  <dimension ref="A1:E1003"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -772,14 +838,14 @@
     <col min="6" max="6" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="7" t="s">
         <v>0</v>
@@ -794,7 +860,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="18" t="s">
         <v>4</v>
@@ -803,7 +869,7 @@
       <c r="D3" s="19"/>
       <c r="E3" s="20"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="10" t="s">
         <v>5</v>
@@ -816,7 +882,7 @@
       </c>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="10" t="s">
         <v>8</v>
@@ -829,7 +895,7 @@
       </c>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="10" t="s">
         <v>10</v>
@@ -844,7 +910,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="10" t="s">
         <v>12</v>
@@ -857,208 +923,227 @@
       </c>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="2"/>
+      <c r="B9" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E9" s="13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="21" t="s">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2"/>
+      <c r="B10" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="23"/>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="23"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
       <c r="B11" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="B12" s="10" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>22</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="B13" s="10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
       <c r="B14" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
       <c r="B15" s="10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
       <c r="B16" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
       <c r="B17" s="10" t="s">
         <v>36</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="2"/>
+      <c r="B18" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D18" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E18" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="10" t="s">
         <v>40</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E20" s="11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="10" t="s">
+    <row r="21" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D21" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E21" s="11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="14" t="s">
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C22" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D22" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="17" t="s">
+      <c r="E22" s="17" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="28"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="28"/>
+    </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2037,10 +2122,12 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>